<commit_message>
Push serializing of Json
Still causes error after second request due to wrong thread in DB. Will attempt to fix
</commit_message>
<xml_diff>
--- a/app/static/database/tables.xlsx
+++ b/app/static/database/tables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Github\2021 Hackathon\app\static\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6AF6EB-19E0-487E-9CD8-55C7045D27D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F6B0C-D4BF-4785-B6A7-0AD90CA20480}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="3" r:id="rId1"/>
-    <sheet name="interests" sheetId="1" r:id="rId2"/>
-    <sheet name="user_interests" sheetId="2" r:id="rId3"/>
+    <sheet name="Interests" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="3" r:id="rId2"/>
+    <sheet name="Messages" sheetId="4" r:id="rId3"/>
+    <sheet name="UserInterests" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,65 +37,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>French</t>
   </si>
   <si>
-    <t>Yoga</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
     <t>Chess</t>
   </si>
   <si>
-    <t>Coding</t>
-  </si>
-  <si>
-    <t>Puzzles</t>
-  </si>
-  <si>
-    <t>Meditation</t>
-  </si>
-  <si>
-    <t>Journaling</t>
-  </si>
-  <si>
     <t>Guitar</t>
   </si>
   <si>
-    <t>Ukulele</t>
-  </si>
-  <si>
-    <t>Saxophone</t>
-  </si>
-  <si>
     <t>Home-Fitness</t>
   </si>
   <si>
-    <t>Baking</t>
-  </si>
-  <si>
-    <t>Aerobics</t>
-  </si>
-  <si>
     <t>Interest</t>
   </si>
   <si>
-    <t>Interest ID</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
     <t>interest</t>
   </si>
   <si>
-    <t>userID</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -123,6 +88,63 @@
   </si>
   <si>
     <t>example_interest</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Hello, any new players?</t>
+  </si>
+  <si>
+    <t>Hi Andrew! I'm brand new at Chess</t>
+  </si>
+  <si>
+    <t>Fancy a game of chess Peter?</t>
+  </si>
+  <si>
+    <t>Sure thing!</t>
+  </si>
+  <si>
+    <t>aerobics</t>
+  </si>
+  <si>
+    <t>french</t>
+  </si>
+  <si>
+    <t>yoga</t>
+  </si>
+  <si>
+    <t>german</t>
+  </si>
+  <si>
+    <t>chess</t>
+  </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>meditation</t>
+  </si>
+  <si>
+    <t>puzzles</t>
+  </si>
+  <si>
+    <t>journaling</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>ukulele</t>
+  </si>
+  <si>
+    <t>saxophone</t>
+  </si>
+  <si>
+    <t>home-fitness</t>
+  </si>
+  <si>
+    <t>baking</t>
   </si>
 </sst>
 </file>
@@ -138,11 +160,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,16 +167,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="MS Shell Dlg 2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,14 +195,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,28 +536,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FFE432-3E07-4FF3-BAA8-D5B2D44624A8}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690216FC-BFE1-4DE1-82EC-8103F2887CE7}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FFE432-3E07-4FF3-BAA8-D5B2D44624A8}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>123</v>
@@ -528,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>123</v>
@@ -539,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>123</v>
@@ -550,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>123</v>
@@ -561,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>123</v>
@@ -572,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>123</v>
@@ -583,149 +771,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690216FC-BFE1-4DE1-82EC-8103F2887CE7}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -735,10 +784,87 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B760FA-28A3-48BD-93C9-58E26331910A}">
+  <dimension ref="D3:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60D84DB-6FAD-4E36-8951-B0FF32DA52AC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -751,38 +877,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Db requests + additional interests
</commit_message>
<xml_diff>
--- a/app/static/database/tables.xlsx
+++ b/app/static/database/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Github\2021 Hackathon\app\static\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F6B0C-D4BF-4785-B6A7-0AD90CA20480}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F23010-0DEF-4A81-BA4B-1719B7FFC8F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
+    <workbookView xWindow="6900" yWindow="3795" windowWidth="19035" windowHeight="11385" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Interests" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690216FC-BFE1-4DE1-82EC-8103F2887CE7}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FFE432-3E07-4FF3-BAA8-D5B2D44624A8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -787,9 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B760FA-28A3-48BD-93C9-58E26331910A}">
   <dimension ref="D3:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -799,7 +797,7 @@
     <col min="7" max="7" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D3" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Push interest updates & ability to pull ids
</commit_message>
<xml_diff>
--- a/app/static/database/tables.xlsx
+++ b/app/static/database/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Github\2021 Hackathon\app\static\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F23010-0DEF-4A81-BA4B-1719B7FFC8F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3530A8D0-B1C0-4BA2-880A-14DF33F431E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="3795" windowWidth="19035" windowHeight="11385" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
+    <workbookView xWindow="31950" yWindow="2760" windowWidth="19035" windowHeight="11385" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Interests" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>French</t>
   </si>
@@ -145,6 +145,84 @@
   </si>
   <si>
     <t>baking</t>
+  </si>
+  <si>
+    <t>drawing</t>
+  </si>
+  <si>
+    <t>sewing</t>
+  </si>
+  <si>
+    <t>cocktails</t>
+  </si>
+  <si>
+    <t>wine-tasting</t>
+  </si>
+  <si>
+    <t>genealogy</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>calligraphy</t>
+  </si>
+  <si>
+    <t>critical thinking</t>
+  </si>
+  <si>
+    <t>poetry</t>
+  </si>
+  <si>
+    <t>youtube creation</t>
+  </si>
+  <si>
+    <t>web design</t>
+  </si>
+  <si>
+    <t>origami</t>
+  </si>
+  <si>
+    <t>entrepreneurship</t>
+  </si>
+  <si>
+    <t>geology</t>
+  </si>
+  <si>
+    <t>stamp collecting</t>
+  </si>
+  <si>
+    <t>candle making</t>
+  </si>
+  <si>
+    <t>jam making</t>
+  </si>
+  <si>
+    <t>knitting</t>
+  </si>
+  <si>
+    <t>goal-setting</t>
+  </si>
+  <si>
+    <t>gaming</t>
+  </si>
+  <si>
+    <t>gardening</t>
+  </si>
+  <si>
+    <t>sudoku</t>
+  </si>
+  <si>
+    <t>breathing exercises</t>
+  </si>
+  <si>
+    <t>comics</t>
+  </si>
+  <si>
+    <t>watercolours</t>
   </si>
 </sst>
 </file>
@@ -537,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690216FC-BFE1-4DE1-82EC-8103F2887CE7}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +745,214 @@
       </c>
       <c r="B15" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Push Capitalised User Interests
</commit_message>
<xml_diff>
--- a/app/static/database/tables.xlsx
+++ b/app/static/database/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Github\2021 Hackathon\app\static\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3530A8D0-B1C0-4BA2-880A-14DF33F431E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315C0804-8F3C-4317-B9CE-15F5D6ACF9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="2760" windowWidth="19035" windowHeight="11385" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CDF2F0C7-9EEF-43D2-A749-0FC2AAA8C8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Interests" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t>French</t>
   </si>
@@ -105,131 +105,182 @@
     <t>Sure thing!</t>
   </si>
   <si>
-    <t>aerobics</t>
-  </si>
-  <si>
-    <t>french</t>
-  </si>
-  <si>
-    <t>yoga</t>
-  </si>
-  <si>
-    <t>german</t>
-  </si>
-  <si>
-    <t>chess</t>
-  </si>
-  <si>
-    <t>coding</t>
-  </si>
-  <si>
-    <t>meditation</t>
-  </si>
-  <si>
-    <t>puzzles</t>
-  </si>
-  <si>
-    <t>journaling</t>
-  </si>
-  <si>
-    <t>guitar</t>
-  </si>
-  <si>
-    <t>ukulele</t>
-  </si>
-  <si>
-    <t>saxophone</t>
-  </si>
-  <si>
-    <t>home-fitness</t>
-  </si>
-  <si>
-    <t>baking</t>
-  </si>
-  <si>
-    <t>drawing</t>
-  </si>
-  <si>
-    <t>sewing</t>
-  </si>
-  <si>
-    <t>cocktails</t>
-  </si>
-  <si>
-    <t>wine-tasting</t>
-  </si>
-  <si>
-    <t>genealogy</t>
-  </si>
-  <si>
-    <t>history</t>
-  </si>
-  <si>
-    <t>reading</t>
-  </si>
-  <si>
-    <t>calligraphy</t>
-  </si>
-  <si>
-    <t>critical thinking</t>
-  </si>
-  <si>
-    <t>poetry</t>
-  </si>
-  <si>
-    <t>youtube creation</t>
-  </si>
-  <si>
-    <t>web design</t>
-  </si>
-  <si>
-    <t>origami</t>
-  </si>
-  <si>
-    <t>entrepreneurship</t>
-  </si>
-  <si>
-    <t>geology</t>
-  </si>
-  <si>
-    <t>stamp collecting</t>
-  </si>
-  <si>
-    <t>candle making</t>
-  </si>
-  <si>
-    <t>jam making</t>
-  </si>
-  <si>
-    <t>knitting</t>
-  </si>
-  <si>
-    <t>goal-setting</t>
-  </si>
-  <si>
-    <t>gaming</t>
-  </si>
-  <si>
-    <t>gardening</t>
-  </si>
-  <si>
-    <t>sudoku</t>
-  </si>
-  <si>
-    <t>breathing exercises</t>
-  </si>
-  <si>
-    <t>comics</t>
-  </si>
-  <si>
-    <t>watercolours</t>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>posted</t>
+  </si>
+  <si>
+    <t>Aerobics</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>Foreign Language</t>
+  </si>
+  <si>
+    <t>Yoga</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Meditation</t>
+  </si>
+  <si>
+    <t>Self-Improvement</t>
+  </si>
+  <si>
+    <t>Puzzles</t>
+  </si>
+  <si>
+    <t>Journaling</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Ukulele</t>
+  </si>
+  <si>
+    <t>Saxophone</t>
+  </si>
+  <si>
+    <t>Baking</t>
+  </si>
+  <si>
+    <t>Food/Drink</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Sewing</t>
+  </si>
+  <si>
+    <t>Practical Skills</t>
+  </si>
+  <si>
+    <t>Cocktails</t>
+  </si>
+  <si>
+    <t>Wine-Tasting</t>
+  </si>
+  <si>
+    <t>Genealogy</t>
+  </si>
+  <si>
+    <t>Knowledge</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Calligraphy</t>
+  </si>
+  <si>
+    <t>Critical Thinking</t>
+  </si>
+  <si>
+    <t>Poetry</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Youtube Creation</t>
+  </si>
+  <si>
+    <t>Hobby</t>
+  </si>
+  <si>
+    <t>Web Design</t>
+  </si>
+  <si>
+    <t>Origami</t>
+  </si>
+  <si>
+    <t>Entrepreneurship</t>
+  </si>
+  <si>
+    <t>Geology</t>
+  </si>
+  <si>
+    <t>Stamp Collecting</t>
+  </si>
+  <si>
+    <t>Candle Making</t>
+  </si>
+  <si>
+    <t>Jam Making</t>
+  </si>
+  <si>
+    <t>Knitting</t>
+  </si>
+  <si>
+    <t>Goal-Setting</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Gardening</t>
+  </si>
+  <si>
+    <t>Sudoku</t>
+  </si>
+  <si>
+    <t>Breathing Exercises</t>
+  </si>
+  <si>
+    <t>Comics</t>
+  </si>
+  <si>
+    <t>Watercolours</t>
+  </si>
+  <si>
+    <t>FortranLover</t>
+  </si>
+  <si>
+    <t>MayoMate99</t>
+  </si>
+  <si>
+    <t>gamerGod14</t>
+  </si>
+  <si>
+    <t>Benny98</t>
+  </si>
+  <si>
+    <t>AlexaSayHi</t>
+  </si>
+  <si>
+    <t>(STARTING WRITING USER INTERESTS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,27 +296,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="MS Shell Dlg 2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -273,33 +313,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,344 +637,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690216FC-BFE1-4DE1-82EC-8103F2887CE7}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -963,19 +1109,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FFE432-3E07-4FF3-BAA8-D5B2D44624A8}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -985,8 +1132,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -996,8 +1156,22 @@
       <c r="C2">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1007,8 +1181,20 @@
       <c r="C3">
         <v>123</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1018,8 +1204,17 @@
       <c r="C4">
         <v>123</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1029,8 +1224,17 @@
       <c r="C5">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1040,8 +1244,17 @@
       <c r="C6">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1051,8 +1264,17 @@
       <c r="C7">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1062,8 +1284,329 @@
       <c r="C8">
         <v>123</v>
       </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9">
+        <v>123</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10">
+        <v>123</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11">
+        <v>123</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12">
+        <v>123</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="O12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13">
+        <v>123</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="O13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="O14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="O16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="O17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="O18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="O19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="O20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="O21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="O22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="O23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="O24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="O25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="O26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="O27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="O28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="O29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>29</v>
+      </c>
+      <c r="O30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>30</v>
+      </c>
+      <c r="O31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>31</v>
+      </c>
+      <c r="O32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="O33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>33</v>
+      </c>
+      <c r="O34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>34</v>
+      </c>
+      <c r="O35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>35</v>
+      </c>
+      <c r="O36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>36</v>
+      </c>
+      <c r="O37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>37</v>
+      </c>
+      <c r="O38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>38</v>
+      </c>
+      <c r="O39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>39</v>
+      </c>
+      <c r="O40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>40</v>
+      </c>
+      <c r="O41" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1071,72 +1614,105 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B760FA-28A3-48BD-93C9-58E26331910A}">
-  <dimension ref="D3:G6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="4:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="4:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="D5" s="2">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="4:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="D6" s="2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="D5" t="s">
         <v>21</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1148,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60D84DB-6FAD-4E36-8951-B0FF32DA52AC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>